<commit_message>
Updates: add all to all membership protocol
</commit_message>
<xml_diff>
--- a/archive/data/leetcode.xlsx
+++ b/archive/data/leetcode.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lingbozh/Desktop/Github/lingbozhang.github.io/archive/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C605BC9D-21CF-C94C-B28E-18813B89CC1E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87FC5E6C-AD16-8645-8197-04A109322B7A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="460" windowWidth="33600" windowHeight="19460" xr2:uid="{E8FB57C8-E8ED-A54A-8AA4-AA4FFB695502}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19420" xr2:uid="{E8FB57C8-E8ED-A54A-8AA4-AA4FFB695502}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -564,8 +564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{909C8600-F738-5146-AEB4-CC849DC044B9}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>